<commit_message>
Some changes in the instruction and #3
</commit_message>
<xml_diff>
--- a/Баллы 2024.xlsx
+++ b/Баллы 2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leon\Student 2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leon\NSTU\Student-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D09CFA-E8D0-4D7E-B0B0-5B89A9E78597}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40EAB86-E809-4A0A-9C23-F12258C49ABF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,7 +146,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,8 +189,14 @@
         <bgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -372,24 +378,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -435,15 +455,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -453,29 +464,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" readingOrder="1"/>
@@ -502,9 +501,52 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1207,1079 +1249,1103 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1:F11"/>
+      <selection pane="topRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10" style="5" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" style="5" customWidth="1"/>
-    <col min="6" max="8" width="14.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="28" style="5" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="39.42578125" style="5" customWidth="1"/>
-    <col min="14" max="17" width="14.28515625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="36.42578125" style="5" customWidth="1"/>
-    <col min="19" max="20" width="14.28515625" style="5" customWidth="1"/>
-    <col min="21" max="21" width="35.5703125" style="5" customWidth="1"/>
-    <col min="22" max="23" width="14.28515625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="38" style="5" customWidth="1"/>
-    <col min="25" max="25" width="14.42578125" style="5" customWidth="1"/>
-    <col min="26" max="26" width="29.140625" style="5" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" style="5"/>
-    <col min="28" max="28" width="9.42578125" style="5" customWidth="1"/>
-    <col min="29" max="30" width="9.28515625" style="5" customWidth="1"/>
-    <col min="31" max="33" width="8.7109375" style="5"/>
-    <col min="34" max="34" width="12.85546875" style="5" customWidth="1"/>
-    <col min="35" max="1024" width="8.7109375" style="5"/>
+    <col min="1" max="1" width="36.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" style="1" customWidth="1"/>
+    <col min="5" max="8" width="14.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="39.42578125" style="1" customWidth="1"/>
+    <col min="14" max="17" width="14.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="36.42578125" style="1" customWidth="1"/>
+    <col min="19" max="20" width="14.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="35.5703125" style="1" customWidth="1"/>
+    <col min="22" max="23" width="14.28515625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="38" style="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="29.140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" style="1"/>
+    <col min="28" max="28" width="9.42578125" style="1" customWidth="1"/>
+    <col min="29" max="30" width="9.28515625" style="1" customWidth="1"/>
+    <col min="31" max="33" width="8.7109375" style="1"/>
+    <col min="34" max="34" width="12.85546875" style="1" customWidth="1"/>
+    <col min="35" max="1024" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="16" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:34" s="12" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9">
+      <c r="C1" s="5">
         <v>44077</v>
       </c>
-      <c r="D1" s="9">
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5">
         <f>C1+7</f>
         <v>44084</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="9">
-        <f>D1+7</f>
+      <c r="F1" s="5">
+        <f>E1+7</f>
         <v>44091</v>
       </c>
-      <c r="G1" s="9">
+      <c r="G1" s="5">
         <f>F1+7</f>
         <v>44098</v>
       </c>
-      <c r="H1" s="9">
+      <c r="H1" s="5">
         <f>G1+7</f>
         <v>44105</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="9">
+      <c r="J1" s="5">
         <f>H1+7</f>
         <v>44112</v>
       </c>
-      <c r="K1" s="9">
+      <c r="K1" s="5">
         <f>J1+7</f>
         <v>44119</v>
       </c>
-      <c r="L1" s="9">
+      <c r="L1" s="5">
         <f>K1+7</f>
         <v>44126</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="9">
+      <c r="N1" s="5">
         <f>L1+7</f>
         <v>44133</v>
       </c>
-      <c r="O1" s="9">
+      <c r="O1" s="5">
         <f>N1+7</f>
         <v>44140</v>
       </c>
-      <c r="P1" s="9">
+      <c r="P1" s="5">
         <f>O1+7</f>
         <v>44147</v>
       </c>
-      <c r="Q1" s="9">
+      <c r="Q1" s="5">
         <f>P1+7</f>
         <v>44154</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="9">
+      <c r="S1" s="5">
         <f>Q1+7</f>
         <v>44161</v>
       </c>
-      <c r="T1" s="9">
+      <c r="T1" s="5">
         <f>S1+7</f>
         <v>44168</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="9">
+      <c r="V1" s="5">
         <f>T1+7</f>
         <v>44175</v>
       </c>
-      <c r="W1" s="9">
+      <c r="W1" s="5">
         <f>V1+7</f>
         <v>44182</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="9">
+      <c r="Y1" s="5">
         <f>W1+7</f>
         <v>44189</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AA1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AB1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AC1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AD1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="AH1" s="17" t="s">
+      <c r="AH1" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" s="14" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="15">
         <v>1</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="34">
         <v>1</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="17">
-        <f>SUM(C2:Z2)</f>
+      <c r="D2" s="35">
+        <v>5</v>
+      </c>
+      <c r="E2" s="35">
         <v>1</v>
       </c>
-      <c r="AB2" s="23" t="str">
-        <f t="shared" ref="AB2:AB11" si="0">IF(AA2&gt;=87,"отл",IF(AA2&gt;=73,"хорошо",IF(AA2&gt;=50,"удовл","Не удовл")))</f>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="13">
+        <f t="shared" ref="AA2:AA11" si="0">SUM(C2:Z2)</f>
+        <v>7</v>
+      </c>
+      <c r="AB2" s="16" t="str">
+        <f t="shared" ref="AB2:AB11" si="1">IF(AA2&gt;=87,"отл",IF(AA2&gt;=73,"хорошо",IF(AA2&gt;=50,"удовл","Не удовл")))</f>
         <v>Не удовл</v>
       </c>
-      <c r="AC2" s="24" t="str">
-        <f t="shared" ref="AC2:AC11" si="1">IF(AA2&gt;=98,"A+",IF(AA2&gt;=93,"A",IF(AA2&gt;=90,"A-",IF(AA2&gt;=87,"B+",IF(AA2&gt;=83,"B",IF(AA2&gt;=80,"B-",IF(AA2&gt;=77,"C+",IF(AA2&gt;=73,"C",IF(AA2&gt;=70,"C-",IF(AA2&gt;=67,"D+",IF(AA2&gt;=63,"D",IF(AA2&gt;=60,"D-",IF(AA2&gt;=50,"E","Не удовл")))))))))))))</f>
+      <c r="AC2" s="17" t="str">
+        <f t="shared" ref="AC2:AC11" si="2">IF(AA2&gt;=98,"A+",IF(AA2&gt;=93,"A",IF(AA2&gt;=90,"A-",IF(AA2&gt;=87,"B+",IF(AA2&gt;=83,"B",IF(AA2&gt;=80,"B-",IF(AA2&gt;=77,"C+",IF(AA2&gt;=73,"C",IF(AA2&gt;=70,"C-",IF(AA2&gt;=67,"D+",IF(AA2&gt;=63,"D",IF(AA2&gt;=60,"D-",IF(AA2&gt;=50,"E","Не удовл")))))))))))))</f>
         <v>Не удовл</v>
       </c>
-      <c r="AD2" s="24" t="str">
-        <f t="shared" ref="AD2:AD11" si="2">IF(AA2&gt;=AH2,"Зачет","Не зачет")</f>
+      <c r="AD2" s="17" t="str">
+        <f t="shared" ref="AD2:AD11" si="3">IF(AA2&gt;=AH2,"Зачет","Не зачет")</f>
         <v>Не зачет</v>
       </c>
-      <c r="AH2" s="17">
+      <c r="AH2" s="13">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:34" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:34" s="14" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="15">
         <v>2</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="34">
         <v>1</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="17">
-        <f>SUM(C3:Z3)</f>
+      <c r="D3" s="35">
+        <v>5</v>
+      </c>
+      <c r="E3" s="35">
         <v>1</v>
       </c>
-      <c r="AB3" s="27" t="str">
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="35"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="13">
         <f t="shared" si="0"/>
-        <v>Не удовл</v>
-      </c>
-      <c r="AC3" s="24" t="str">
+        <v>7</v>
+      </c>
+      <c r="AB3" s="19" t="str">
         <f t="shared" si="1"/>
         <v>Не удовл</v>
       </c>
-      <c r="AD3" s="24" t="str">
+      <c r="AC3" s="17" t="str">
         <f t="shared" si="2"/>
+        <v>Не удовл</v>
+      </c>
+      <c r="AD3" s="17" t="str">
+        <f t="shared" si="3"/>
         <v>Не зачет</v>
       </c>
-      <c r="AH3" s="17">
+      <c r="AH3" s="13">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:34" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" s="14" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="15">
         <v>3</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="34">
         <v>0.5</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="17">
-        <f>SUM(C4:Z4)</f>
-        <v>0.5</v>
-      </c>
-      <c r="AB4" s="28" t="str">
+      <c r="D4" s="35">
+        <v>5</v>
+      </c>
+      <c r="E4" s="35">
+        <v>1</v>
+      </c>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="35"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="13">
         <f t="shared" si="0"/>
-        <v>Не удовл</v>
-      </c>
-      <c r="AC4" s="24" t="str">
+        <v>6.5</v>
+      </c>
+      <c r="AB4" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Не удовл</v>
       </c>
-      <c r="AD4" s="24" t="str">
+      <c r="AC4" s="17" t="str">
         <f t="shared" si="2"/>
+        <v>Не удовл</v>
+      </c>
+      <c r="AD4" s="17" t="str">
+        <f t="shared" si="3"/>
         <v>Не зачет</v>
       </c>
-      <c r="AH4" s="17">
+      <c r="AH4" s="13">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:34" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+    <row r="5" spans="1:34" s="14" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="15">
         <v>4</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="34">
         <v>1</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="22"/>
-      <c r="AA5" s="17">
-        <f>SUM(C5:Z5)</f>
+      <c r="D5" s="35">
+        <v>5</v>
+      </c>
+      <c r="E5" s="35">
         <v>1</v>
       </c>
-      <c r="AB5" s="28" t="str">
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="38"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="36"/>
+      <c r="AA5" s="13">
         <f t="shared" si="0"/>
-        <v>Не удовл</v>
-      </c>
-      <c r="AC5" s="24" t="str">
+        <v>7</v>
+      </c>
+      <c r="AB5" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Не удовл</v>
       </c>
-      <c r="AD5" s="24" t="str">
+      <c r="AC5" s="17" t="str">
         <f t="shared" si="2"/>
+        <v>Не удовл</v>
+      </c>
+      <c r="AD5" s="17" t="str">
+        <f t="shared" si="3"/>
         <v>Не зачет</v>
       </c>
-      <c r="AH5" s="17">
+      <c r="AH5" s="13">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:34" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:34" s="14" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="15">
         <v>5</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="34">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="17">
-        <f>SUM(C6:Z6)</f>
+      <c r="D6" s="35">
+        <v>5</v>
+      </c>
+      <c r="E6" s="35">
         <v>1</v>
       </c>
-      <c r="AB6" s="28" t="str">
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="13">
         <f t="shared" si="0"/>
-        <v>Не удовл</v>
-      </c>
-      <c r="AC6" s="24" t="str">
+        <v>7</v>
+      </c>
+      <c r="AB6" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Не удовл</v>
       </c>
-      <c r="AD6" s="24" t="str">
+      <c r="AC6" s="17" t="str">
         <f t="shared" si="2"/>
+        <v>Не удовл</v>
+      </c>
+      <c r="AD6" s="17" t="str">
+        <f t="shared" si="3"/>
         <v>Не зачет</v>
       </c>
-      <c r="AH6" s="17">
+      <c r="AH6" s="13">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:34" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:34" s="14" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="15">
         <v>6</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="34">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="17">
-        <f>SUM(C7:Z7)</f>
+      <c r="D7" s="35">
+        <v>5</v>
+      </c>
+      <c r="E7" s="35">
         <v>1</v>
       </c>
-      <c r="AB7" s="28" t="str">
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="37"/>
+      <c r="AA7" s="13">
         <f t="shared" si="0"/>
-        <v>Не удовл</v>
-      </c>
-      <c r="AC7" s="24" t="str">
+        <v>7</v>
+      </c>
+      <c r="AB7" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Не удовл</v>
       </c>
-      <c r="AD7" s="24" t="str">
+      <c r="AC7" s="17" t="str">
         <f t="shared" si="2"/>
+        <v>Не удовл</v>
+      </c>
+      <c r="AD7" s="17" t="str">
+        <f t="shared" si="3"/>
         <v>Не зачет</v>
       </c>
-      <c r="AH7" s="17">
+      <c r="AH7" s="13">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:34" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30"/>
-      <c r="B8" s="19">
+    <row r="8" spans="1:34" s="14" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21"/>
+      <c r="B8" s="15">
         <v>7</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="26"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="17">
-        <f>SUM(C8:Z8)</f>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="37"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="36"/>
+      <c r="AA8" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB8" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v>Не удовл</v>
-      </c>
-      <c r="AC8" s="24" t="str">
+      <c r="AB8" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Не удовл</v>
       </c>
-      <c r="AD8" s="24" t="str">
+      <c r="AC8" s="17" t="str">
         <f t="shared" si="2"/>
+        <v>Не удовл</v>
+      </c>
+      <c r="AD8" s="17" t="str">
+        <f t="shared" si="3"/>
         <v>Не зачет</v>
       </c>
-      <c r="AH8" s="17">
+      <c r="AH8" s="13">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:34" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="19">
+    <row r="9" spans="1:34" s="14" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="15">
         <v>8</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
-      <c r="Y9" s="29"/>
-      <c r="Z9" s="33"/>
-      <c r="AA9" s="17">
-        <f>SUM(C9:Z9)</f>
+      <c r="C9" s="39"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="40"/>
+      <c r="AA9" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB9" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v>Не удовл</v>
-      </c>
-      <c r="AC9" s="24" t="str">
+      <c r="AB9" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Не удовл</v>
       </c>
-      <c r="AD9" s="24" t="str">
+      <c r="AC9" s="17" t="str">
         <f t="shared" si="2"/>
+        <v>Не удовл</v>
+      </c>
+      <c r="AD9" s="17" t="str">
+        <f t="shared" si="3"/>
         <v>Не зачет</v>
       </c>
-      <c r="AH9" s="17">
+      <c r="AH9" s="13">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:34" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
-      <c r="B10" s="19">
+    <row r="10" spans="1:34" s="14" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
+      <c r="B10" s="15">
         <v>9</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="22"/>
-      <c r="AA10" s="17">
-        <f>SUM(C10:Z10)</f>
+      <c r="C10" s="34"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
+      <c r="X10" s="35"/>
+      <c r="Y10" s="35"/>
+      <c r="Z10" s="36"/>
+      <c r="AA10" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB10" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v>Не удовл</v>
-      </c>
-      <c r="AC10" s="24" t="str">
+      <c r="AB10" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Не удовл</v>
       </c>
-      <c r="AD10" s="24" t="str">
+      <c r="AC10" s="17" t="str">
         <f t="shared" si="2"/>
+        <v>Не удовл</v>
+      </c>
+      <c r="AD10" s="17" t="str">
+        <f t="shared" si="3"/>
         <v>Не зачет</v>
       </c>
-      <c r="AH10" s="17">
+      <c r="AH10" s="13">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:34" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
-      <c r="B11" s="19">
+    <row r="11" spans="1:34" s="14" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21"/>
+      <c r="B11" s="15">
         <v>10</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="34">
-        <f>SUM(C11:Z11)</f>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35"/>
+      <c r="X11" s="37"/>
+      <c r="Y11" s="35"/>
+      <c r="Z11" s="37"/>
+      <c r="AA11" s="23">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB11" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v>Не удовл</v>
-      </c>
-      <c r="AC11" s="24" t="str">
+      <c r="AB11" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Не удовл</v>
       </c>
-      <c r="AD11" s="24" t="str">
+      <c r="AC11" s="17" t="str">
         <f t="shared" si="2"/>
+        <v>Не удовл</v>
+      </c>
+      <c r="AD11" s="17" t="str">
+        <f t="shared" si="3"/>
         <v>Не зачет</v>
       </c>
-      <c r="AH11" s="34">
+      <c r="AH11" s="23">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:34" s="39" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="4" t="s">
+    <row r="12" spans="1:34" s="28" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="45"/>
+      <c r="E12" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="2" t="s">
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2" t="s">
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2" t="s">
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="4" t="s">
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="1" t="s">
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="17"/>
-      <c r="AB12" s="37"/>
-      <c r="AC12" s="38"/>
-      <c r="AD12" s="38"/>
-      <c r="AH12" s="40"/>
+      <c r="Z12" s="42"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="27"/>
+      <c r="AD12" s="27"/>
+      <c r="AH12" s="29"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="41"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="41"/>
-      <c r="AH13" s="41"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="30"/>
+      <c r="AA13" s="30"/>
+      <c r="AH13" s="30"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="43"/>
-      <c r="Q14" s="43"/>
-      <c r="R14" s="43"/>
-      <c r="S14" s="43"/>
-      <c r="T14" s="43"/>
-      <c r="U14" s="43"/>
-      <c r="V14" s="43"/>
-      <c r="W14" s="43"/>
-      <c r="X14" s="43"/>
-      <c r="Y14" s="43"/>
-      <c r="Z14" s="43"/>
-      <c r="AA14" s="43"/>
-      <c r="AH14" s="43"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="32"/>
+      <c r="AH14" s="32"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="43"/>
-      <c r="R15" s="43"/>
-      <c r="S15" s="43"/>
-      <c r="T15" s="43"/>
-      <c r="U15" s="43"/>
-      <c r="V15" s="43"/>
-      <c r="W15" s="43"/>
-      <c r="X15" s="43"/>
-      <c r="Y15" s="43"/>
-      <c r="Z15" s="43"/>
-      <c r="AA15" s="43"/>
-      <c r="AH15" s="43"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="32"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="32"/>
+      <c r="Y15" s="32"/>
+      <c r="Z15" s="32"/>
+      <c r="AA15" s="32"/>
+      <c r="AH15" s="32"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="43"/>
-      <c r="T16" s="43"/>
-      <c r="U16" s="43"/>
-      <c r="V16" s="43"/>
-      <c r="W16" s="43"/>
-      <c r="X16" s="43"/>
-      <c r="Y16" s="43"/>
-      <c r="Z16" s="43"/>
-      <c r="AA16" s="43"/>
-      <c r="AH16" s="43"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="32"/>
+      <c r="Z16" s="32"/>
+      <c r="AA16" s="32"/>
+      <c r="AH16" s="32"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
-      <c r="R17" s="43"/>
-      <c r="S17" s="43"/>
-      <c r="T17" s="43"/>
-      <c r="U17" s="43"/>
-      <c r="V17" s="43"/>
-      <c r="W17" s="43"/>
-      <c r="X17" s="43"/>
-      <c r="Y17" s="43"/>
-      <c r="Z17" s="43"/>
-      <c r="AA17" s="43"/>
-      <c r="AH17" s="43"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="32"/>
+      <c r="AA17" s="32"/>
+      <c r="AH17" s="32"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="J18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="43"/>
-      <c r="R18" s="43"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="43"/>
-      <c r="U18" s="43"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="43"/>
-      <c r="X18" s="43"/>
-      <c r="Y18" s="43"/>
-      <c r="Z18" s="43"/>
-      <c r="AA18" s="43"/>
-      <c r="AH18" s="43"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="J18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="32"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="32"/>
+      <c r="Z18" s="32"/>
+      <c r="AA18" s="32"/>
+      <c r="AH18" s="32"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="J19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="43"/>
-      <c r="R19" s="43"/>
-      <c r="S19" s="43"/>
-      <c r="T19" s="43"/>
-      <c r="U19" s="43"/>
-      <c r="V19" s="43"/>
-      <c r="W19" s="43"/>
-      <c r="X19" s="43"/>
-      <c r="Y19" s="43"/>
-      <c r="Z19" s="43"/>
-      <c r="AA19" s="43"/>
-      <c r="AH19" s="43"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="J19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="32"/>
+      <c r="Z19" s="32"/>
+      <c r="AA19" s="32"/>
+      <c r="AH19" s="32"/>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="J20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="43"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="43"/>
-      <c r="T20" s="43"/>
-      <c r="U20" s="43"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="43"/>
-      <c r="X20" s="43"/>
-      <c r="Y20" s="43"/>
-      <c r="Z20" s="43"/>
-      <c r="AA20" s="43"/>
-      <c r="AH20" s="43"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="J20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="32"/>
+      <c r="Z20" s="32"/>
+      <c r="AA20" s="32"/>
+      <c r="AH20" s="32"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="J21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="43"/>
-      <c r="S21" s="43"/>
-      <c r="T21" s="43"/>
-      <c r="U21" s="43"/>
-      <c r="V21" s="43"/>
-      <c r="W21" s="43"/>
-      <c r="X21" s="43"/>
-      <c r="Y21" s="43"/>
-      <c r="Z21" s="43"/>
-      <c r="AA21" s="43"/>
-      <c r="AH21" s="43"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="J21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="32"/>
+      <c r="Z21" s="32"/>
+      <c r="AA21" s="32"/>
+      <c r="AH21" s="32"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="J22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="43"/>
-      <c r="Q22" s="43"/>
-      <c r="R22" s="43"/>
-      <c r="S22" s="43"/>
-      <c r="T22" s="43"/>
-      <c r="U22" s="43"/>
-      <c r="V22" s="43"/>
-      <c r="W22" s="43"/>
-      <c r="X22" s="43"/>
-      <c r="Y22" s="43"/>
-      <c r="Z22" s="43"/>
-      <c r="AA22" s="43"/>
-      <c r="AH22" s="43"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="J22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="32"/>
+      <c r="Z22" s="32"/>
+      <c r="AA22" s="32"/>
+      <c r="AH22" s="32"/>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="J23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="43"/>
-      <c r="T23" s="43"/>
-      <c r="U23" s="43"/>
-      <c r="V23" s="43"/>
-      <c r="W23" s="43"/>
-      <c r="X23" s="43"/>
-      <c r="Y23" s="43"/>
-      <c r="Z23" s="43"/>
-      <c r="AA23" s="43"/>
-      <c r="AH23" s="43"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="J23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="32"/>
+      <c r="Y23" s="32"/>
+      <c r="Z23" s="32"/>
+      <c r="AA23" s="32"/>
+      <c r="AH23" s="32"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="J24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="43"/>
-      <c r="T24" s="43"/>
-      <c r="U24" s="43"/>
-      <c r="V24" s="43"/>
-      <c r="W24" s="43"/>
-      <c r="X24" s="43"/>
-      <c r="Y24" s="43"/>
-      <c r="Z24" s="43"/>
-      <c r="AA24" s="43"/>
-      <c r="AH24" s="43"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="J24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="32"/>
+      <c r="S24" s="32"/>
+      <c r="T24" s="32"/>
+      <c r="U24" s="32"/>
+      <c r="V24" s="32"/>
+      <c r="W24" s="32"/>
+      <c r="X24" s="32"/>
+      <c r="Y24" s="32"/>
+      <c r="Z24" s="32"/>
+      <c r="AA24" s="32"/>
+      <c r="AH24" s="32"/>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="J25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="43"/>
-      <c r="T25" s="43"/>
-      <c r="U25" s="43"/>
-      <c r="V25" s="43"/>
-      <c r="W25" s="43"/>
-      <c r="X25" s="43"/>
-      <c r="Y25" s="43"/>
-      <c r="Z25" s="43"/>
-      <c r="AA25" s="43"/>
-      <c r="AH25" s="43"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="J25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="32"/>
+      <c r="Z25" s="32"/>
+      <c r="AA25" s="32"/>
+      <c r="AH25" s="32"/>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="J26" s="5"/>
-      <c r="L26" s="5"/>
+      <c r="J26" s="1"/>
+      <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="J27" s="5"/>
-      <c r="L27" s="5"/>
+      <c r="J27" s="1"/>
+      <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="J28" s="5"/>
-      <c r="L28" s="5"/>
+      <c r="J28" s="1"/>
+      <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="J29" s="5"/>
-      <c r="L29" s="5"/>
+      <c r="J29" s="1"/>
+      <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="J30" s="5"/>
-      <c r="L30" s="5"/>
+      <c r="J30" s="1"/>
+      <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="J31" s="5"/>
-      <c r="L31" s="5"/>
+      <c r="J31" s="1"/>
+      <c r="L31" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/+vyCLhbrGGgMz70Qt4UMZbWVBuie06HlMLk0OyolQ75CT5RwNOQrTqSslAIpSA5HmPYfAh+DZjmC8KjfKGphA==" saltValue="TjeFtoy5OVu/5r0QuvzmoA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="qSouQdbU//enmv3FQZGUFLbMg9ML28z0T+Dfaej5gieh+6fsojHkhCJc1m6GZNmwhT4z194AMhQ4pWm5pgL7Lg==" saltValue="kqgUBfwgkt1Af92RfaeEdA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:I12"/>
     <mergeCell ref="V12:X12"/>
     <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:I12"/>
     <mergeCell ref="J12:M12"/>
     <mergeCell ref="N12:R12"/>
     <mergeCell ref="S12:U12"/>
   </mergeCells>
-  <conditionalFormatting sqref="R2:R7">
+  <conditionalFormatting sqref="R2:R7 D10:J11 D2:M3 C2:C11 D4:H9">
     <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2309,7 +2375,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:J11 C2:M3 K5:M7 P2:Q7 W7:Y7 W5:Z6 C4:H9 I5:J9 I4:M4 W3:Y4 W2:Z2 T5:T7 T2:U4">
+  <conditionalFormatting sqref="K5:M7 P2:Q7 W7:Y7 W5:Z6 I5:J9 I4:M4 W3:Y4 W2:Z2 T5:T7 T2:U4">
     <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2469,7 +2535,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update tasks and points
</commit_message>
<xml_diff>
--- a/Баллы 2024.xlsx
+++ b/Баллы 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leon\NSTU\Student-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB49E630-11F1-4507-8E03-5AEE4C99563E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1456F9FB-AD05-4476-B836-4CB52748A473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="2565" windowWidth="27030" windowHeight="15690" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38835" yWindow="3810" windowWidth="26145" windowHeight="16140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Группа ФТ-61М</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t xml:space="preserve">Копылов Александр Дмитриевич </t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1045,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I2" sqref="I2"/>
+      <selection pane="topRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,9 +1212,15 @@
       <c r="H2" s="31">
         <v>1</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+      <c r="I2" s="31">
+        <v>7</v>
+      </c>
+      <c r="J2" s="31">
+        <v>1</v>
+      </c>
+      <c r="K2" s="31">
+        <v>1</v>
+      </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
       <c r="N2" s="31"/>
@@ -1229,7 +1238,7 @@
       <c r="Z2" s="32"/>
       <c r="AA2" s="13">
         <f t="shared" ref="AA2:AA11" si="0">SUM(C2:Z2)</f>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="AB2" s="16" t="str">
         <f t="shared" ref="AB2:AB11" si="1">IF(AA2&gt;=87,"отл",IF(AA2&gt;=73,"хорошо",IF(AA2&gt;=50,"удовл","Не удовл")))</f>
@@ -1276,7 +1285,9 @@
         <v>8</v>
       </c>
       <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
+      <c r="K3" s="31">
+        <v>1</v>
+      </c>
       <c r="L3" s="31"/>
       <c r="M3" s="31"/>
       <c r="N3" s="31"/>
@@ -1294,7 +1305,7 @@
       <c r="Z3" s="33"/>
       <c r="AA3" s="13">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AB3" s="19" t="str">
         <f t="shared" si="1"/>
@@ -1340,8 +1351,12 @@
       <c r="I4" s="31">
         <v>8</v>
       </c>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
+      <c r="J4" s="31">
+        <v>1</v>
+      </c>
+      <c r="K4" s="31">
+        <v>1</v>
+      </c>
       <c r="L4" s="31"/>
       <c r="M4" s="31"/>
       <c r="N4" s="31"/>
@@ -1359,7 +1374,7 @@
       <c r="Z4" s="33"/>
       <c r="AA4" s="13">
         <f t="shared" si="0"/>
-        <v>17.5</v>
+        <v>19.5</v>
       </c>
       <c r="AB4" s="20" t="str">
         <f t="shared" si="1"/>
@@ -1405,10 +1420,16 @@
       <c r="I5" s="31">
         <v>8</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
+      <c r="J5" s="31">
+        <v>1</v>
+      </c>
+      <c r="K5" s="31">
+        <v>1</v>
+      </c>
       <c r="L5" s="31"/>
-      <c r="M5" s="34"/>
+      <c r="M5" s="34">
+        <v>11</v>
+      </c>
       <c r="N5" s="31"/>
       <c r="O5" s="31"/>
       <c r="P5" s="31"/>
@@ -1424,7 +1445,7 @@
       <c r="Z5" s="32"/>
       <c r="AA5" s="13">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="AB5" s="20" t="str">
         <f t="shared" si="1"/>
@@ -1471,9 +1492,13 @@
         <v>8</v>
       </c>
       <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
+      <c r="K6" s="31">
+        <v>1</v>
+      </c>
       <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
+      <c r="M6" s="31" t="s">
+        <v>26</v>
+      </c>
       <c r="N6" s="31"/>
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
@@ -1489,7 +1514,7 @@
       <c r="Z6" s="32"/>
       <c r="AA6" s="13">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AB6" s="20" t="str">
         <f t="shared" si="1"/>
@@ -1535,10 +1560,16 @@
       <c r="I7" s="31">
         <v>8</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
+      <c r="J7" s="31">
+        <v>1</v>
+      </c>
+      <c r="K7" s="31">
+        <v>1</v>
+      </c>
       <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
+      <c r="M7" s="31" t="s">
+        <v>26</v>
+      </c>
       <c r="N7" s="31"/>
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
@@ -1554,7 +1585,7 @@
       <c r="Z7" s="33"/>
       <c r="AA7" s="13">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AB7" s="20" t="str">
         <f t="shared" si="1"/>
@@ -2174,7 +2205,7 @@
       <c r="L31" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gXf646W3K3ba50+g7vDUOkbiWO/94n6W4MVi/uFcbN3TUnJJwhE2ePmLn8JFj9e1nXzF0fNFPsYWZ4sgQOfM4Q==" saltValue="3VJb8N02ekJh4B6dEGiHmw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kyPQhY3RRDqlLVvLsRkAW43vhEq9eNqR9mAAQGRepCM8upxgkPl6kUe49BEUeuL7IZ79dR2upIBOPkLITuL5PQ==" saltValue="DLTKiPBLIhoFU0WBmMUrDQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:I12"/>

</xml_diff>